<commit_message>
删除无效文件 Co-authored-by: shiyuq <1543082564@qq.com>
</commit_message>
<xml_diff>
--- a/sample-file/product.xlsx
+++ b/sample-file/product.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\qcc\workspace\know-your-quotation\sample-file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9B9835-3607-4D1B-8D18-1987B9D7C64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6787FFD-A283-4344-BA6C-A24CE3747E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-15" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,10 +71,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OK1013</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ACT1013-2.5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -119,10 +115,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OK9100B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>RBK9100B</t>
   </si>
   <si>
@@ -139,10 +131,6 @@
   </si>
   <si>
     <t>RBK1224-244-O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OK1224</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -208,6 +196,18 @@
   </si>
   <si>
     <t>序号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEST1013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEST9100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEST1224</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -264,7 +264,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -274,6 +274,9 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -698,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -721,7 +724,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -742,13 +745,13 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>3</v>
@@ -766,28 +769,28 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="G2" s="1">
         <v>2.5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1">
         <v>2.5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>8</v>
@@ -807,22 +810,22 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="1">
         <v>5</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="1">
         <v>5</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>8</v>
@@ -842,22 +845,22 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1">
         <v>7.5</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" s="1">
         <v>7.5</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>8</v>
@@ -877,22 +880,22 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1">
         <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="1">
         <v>10</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>8</v>
@@ -909,31 +912,31 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="I6" s="1">
         <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L6" s="1">
         <v>73</v>
@@ -948,31 +951,31 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="I7" s="1">
         <v>1.5</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L7" s="1">
         <v>80</v>
@@ -989,25 +992,25 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I8" s="1">
         <v>2.5</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L8" s="1">
         <v>120</v>
@@ -1024,25 +1027,25 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I9" s="1">
         <v>3.5</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L9" s="1">
         <v>160</v>

</xml_diff>